<commit_message>
Add explanation_nb and wordclass to the test doc
</commit_message>
<xml_diff>
--- a/termwikiimporter/test/excel/simple.xlsx
+++ b/termwikiimporter/test/excel/simple.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>fi</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>Dette er forklaringen</t>
   </si>
 </sst>
 </file>
@@ -137,16 +140,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="191" zoomScaleNormal="191" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -172,6 +172,9 @@
       <c r="D2" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="E2" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>